<commit_message>
data cleaning Q3 - V03
</commit_message>
<xml_diff>
--- a/tech_layoffs_csv/Layoffs.fyi Tracker_Q3_2024.xlsx
+++ b/tech_layoffs_csv/Layoffs.fyi Tracker_Q3_2024.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrike_imac_air/projects/DataScienceProjects/tech_layoffs_project/tech_layoffs_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2760D60-22EA-2E46-8391-1E314A18BED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ABADDC-25B1-A649-B55C-DAE1F4AB493C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="860" windowWidth="29780" windowHeight="22440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$140</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="270">
   <si>
     <r>
       <rPr>
@@ -2781,6 +2784,51 @@
   </si>
   <si>
     <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Foster City</t>
+  </si>
+  <si>
+    <t>Campbell</t>
+  </si>
+  <si>
+    <t>Menlo Park</t>
+  </si>
+  <si>
+    <t>Cupertino</t>
+  </si>
+  <si>
+    <t>Fremont</t>
+  </si>
+  <si>
+    <t>San Ramon</t>
+  </si>
+  <si>
+    <t>San Mateo</t>
+  </si>
+  <si>
+    <t>Palo Alto</t>
+  </si>
+  <si>
+    <t>Walnut Creek</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>Santa Clara</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Mountain View</t>
+  </si>
+  <si>
+    <t>Berkeley</t>
+  </si>
+  <si>
+    <t>San Francisco Bay Area</t>
   </si>
 </sst>
 </file>
@@ -2983,7 +3031,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3061,6 +3109,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3368,16 +3419,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F364D8-7C39-9F42-8917-7C47B6C1B156}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R140"/>
+  <dimension ref="A1:R147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="L117" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P140" sqref="A2:P140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="11"/>
-    <col min="2" max="2" width="17.19921875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" style="11" customWidth="1"/>
     <col min="3" max="5" width="31.3984375" style="11" customWidth="1"/>
     <col min="6" max="6" width="23" style="22" customWidth="1"/>
     <col min="7" max="7" width="31.3984375" style="11" customWidth="1"/>
@@ -3799,9 +3850,11 @@
         <v>57</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D11" s="14"/>
+        <v>255</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="18" t="s">
         <v>36</v>
@@ -3875,7 +3928,7 @@
       <c r="C13" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="21"/>
       <c r="F13" s="15" t="s">
         <v>19</v>
@@ -3913,7 +3966,7 @@
       <c r="C14" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="13"/>
       <c r="F14" s="15" t="s">
         <v>20</v>
@@ -3949,7 +4002,7 @@
       <c r="C15" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="21"/>
       <c r="F15" s="18" t="s">
         <v>36</v>
@@ -3983,7 +4036,7 @@
       <c r="C16" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="21"/>
       <c r="F16" s="15" t="s">
         <v>21</v>
@@ -4095,7 +4148,9 @@
       <c r="C19" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E19" s="14"/>
       <c r="F19" s="18" t="s">
         <v>36</v>
@@ -4171,7 +4226,7 @@
       <c r="C21" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="13"/>
       <c r="F21" s="15" t="s">
         <v>20</v>
@@ -4315,7 +4370,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -4361,9 +4416,11 @@
         <v>79</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D26" s="14"/>
+        <v>256</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E26" s="14"/>
       <c r="F26" s="18" t="s">
         <v>36</v>
@@ -4441,7 +4498,9 @@
       <c r="C28" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E28" s="14"/>
       <c r="F28" s="18" t="s">
         <v>36</v>
@@ -4517,7 +4576,7 @@
       <c r="C30" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="13"/>
       <c r="F30" s="15" t="s">
         <v>24</v>
@@ -4631,9 +4690,11 @@
         <v>91</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D33" s="14"/>
+        <v>257</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E33" s="14"/>
       <c r="F33" s="18" t="s">
         <v>36</v>
@@ -4673,7 +4734,9 @@
       <c r="C34" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D34" s="14"/>
+      <c r="D34" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E34" s="14"/>
       <c r="F34" s="18" t="s">
         <v>36</v>
@@ -4711,9 +4774,11 @@
         <v>94</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D35" s="14"/>
+        <v>258</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E35" s="14"/>
       <c r="F35" s="18" t="s">
         <v>36</v>
@@ -4751,7 +4816,7 @@
       <c r="C36" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="13"/>
       <c r="F36" s="15" t="s">
         <v>25</v>
@@ -4777,7 +4842,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -4825,9 +4890,11 @@
         <v>96</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D38" s="14"/>
+        <v>259</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E38" s="14"/>
       <c r="F38" s="18" t="s">
         <v>36</v>
@@ -4865,7 +4932,7 @@
       <c r="C39" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="D39" s="13"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="13"/>
       <c r="F39" s="15" t="s">
         <v>20</v>
@@ -4903,7 +4970,7 @@
       <c r="C40" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D40" s="21"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="21"/>
       <c r="F40" s="18" t="s">
         <v>36</v>
@@ -4939,7 +5006,7 @@
       <c r="C41" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="5"/>
       <c r="F41" s="15" t="s">
         <v>19</v>
@@ -5015,7 +5082,7 @@
       <c r="C43" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="21"/>
       <c r="F43" s="18" t="s">
         <v>36</v>
@@ -5089,9 +5156,11 @@
         <v>104</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="14"/>
+        <v>260</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E45" s="14"/>
       <c r="F45" s="18" t="s">
         <v>36</v>
@@ -5167,9 +5236,11 @@
         <v>107</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D47" s="14"/>
+        <v>261</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E47" s="14"/>
       <c r="F47" s="18" t="s">
         <v>36</v>
@@ -5209,7 +5280,7 @@
       <c r="C48" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D48" s="21"/>
+      <c r="D48" s="14"/>
       <c r="E48" s="21"/>
       <c r="F48" s="18" t="s">
         <v>36</v>
@@ -5245,7 +5316,7 @@
       <c r="C49" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="13"/>
       <c r="F49" s="15" t="s">
         <v>19</v>
@@ -5393,9 +5464,11 @@
         <v>113</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D53" s="14"/>
+        <v>262</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E53" s="14"/>
       <c r="F53" s="18" t="s">
         <v>36</v>
@@ -5433,7 +5506,7 @@
       <c r="C54" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="D54" s="13"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="13"/>
       <c r="F54" s="15" t="s">
         <v>22</v>
@@ -5509,7 +5582,7 @@
       <c r="C56" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D56" s="13"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="13"/>
       <c r="F56" s="15" t="s">
         <v>24</v>
@@ -5583,7 +5656,7 @@
       <c r="C58" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="D58" s="5"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="5"/>
       <c r="F58" s="15" t="s">
         <v>19</v>
@@ -5659,9 +5732,11 @@
         <v>121</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D60" s="14"/>
+        <v>257</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E60" s="14"/>
       <c r="F60" s="18" t="s">
         <v>36</v>
@@ -5695,9 +5770,11 @@
         <v>122</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D61" s="14"/>
+        <v>263</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E61" s="14"/>
       <c r="F61" s="18" t="s">
         <v>36</v>
@@ -5735,7 +5812,7 @@
       <c r="C62" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="D62" s="13"/>
+      <c r="D62" s="14"/>
       <c r="E62" s="13"/>
       <c r="F62" s="15" t="s">
         <v>26</v>
@@ -5771,7 +5848,9 @@
       <c r="C63" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D63" s="14"/>
+      <c r="D63" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E63" s="14"/>
       <c r="F63" s="18" t="s">
         <v>36</v>
@@ -5807,9 +5886,11 @@
         <v>125</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D64" s="14"/>
+        <v>264</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E64" s="14"/>
       <c r="F64" s="18" t="s">
         <v>36</v>
@@ -5847,9 +5928,11 @@
         <v>126</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D65" s="14"/>
+        <v>262</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E65" s="14"/>
       <c r="F65" s="18" t="s">
         <v>36</v>
@@ -5961,7 +6044,9 @@
       <c r="C68" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D68" s="14"/>
+      <c r="D68" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E68" s="14"/>
       <c r="F68" s="18" t="s">
         <v>36</v>
@@ -5999,7 +6084,9 @@
       <c r="C69" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D69" s="14"/>
+      <c r="D69" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E69" s="14"/>
       <c r="F69" s="18" t="s">
         <v>36</v>
@@ -6077,7 +6164,7 @@
       <c r="C71" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="D71" s="21"/>
+      <c r="D71" s="14"/>
       <c r="E71" s="21"/>
       <c r="F71" s="18" t="s">
         <v>36</v>
@@ -6117,7 +6204,7 @@
       <c r="C72" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="D72" s="13"/>
+      <c r="D72" s="14"/>
       <c r="E72" s="13"/>
       <c r="F72" s="15" t="s">
         <v>27</v>
@@ -6191,7 +6278,7 @@
       <c r="C74" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="D74" s="13"/>
+      <c r="D74" s="14"/>
       <c r="E74" s="13"/>
       <c r="F74" s="15" t="s">
         <v>24</v>
@@ -6341,9 +6428,11 @@
         <v>144</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D78" s="14"/>
+        <v>265</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E78" s="14"/>
       <c r="F78" s="18" t="s">
         <v>36</v>
@@ -6373,7 +6462,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="30" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A79" s="12">
         <v>78</v>
       </c>
@@ -6459,7 +6548,7 @@
       <c r="C81" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D81" s="13"/>
+      <c r="D81" s="14"/>
       <c r="E81" s="13"/>
       <c r="F81" s="15" t="s">
         <v>24</v>
@@ -6497,7 +6586,7 @@
       <c r="C82" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D82" s="21"/>
+      <c r="D82" s="14"/>
       <c r="E82" s="21"/>
       <c r="F82" s="18" t="s">
         <v>36</v>
@@ -6533,7 +6622,9 @@
       <c r="C83" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D83" s="14"/>
+      <c r="D83" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E83" s="14"/>
       <c r="F83" s="18" t="s">
         <v>36</v>
@@ -6569,9 +6660,11 @@
         <v>150</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D84" s="14"/>
+        <v>266</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E84" s="14"/>
       <c r="F84" s="18" t="s">
         <v>36</v>
@@ -6685,7 +6778,7 @@
       <c r="C87" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D87" s="13"/>
+      <c r="D87" s="14"/>
       <c r="E87" s="13"/>
       <c r="F87" s="15" t="s">
         <v>20</v>
@@ -6723,7 +6816,9 @@
       <c r="C88" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D88" s="14"/>
+      <c r="D88" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E88" s="14"/>
       <c r="F88" s="18" t="s">
         <v>36</v>
@@ -6761,7 +6856,9 @@
       <c r="C89" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D89" s="14"/>
+      <c r="D89" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E89" s="14"/>
       <c r="F89" s="18" t="s">
         <v>36</v>
@@ -6801,7 +6898,7 @@
       <c r="C90" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="D90" s="5"/>
+      <c r="D90" s="14"/>
       <c r="E90" s="5"/>
       <c r="F90" s="15" t="s">
         <v>19</v>
@@ -6911,13 +7008,15 @@
       <c r="A93" s="12">
         <v>92</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="26" t="s">
         <v>159</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D93" s="14"/>
+        <v>262</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E93" s="14"/>
       <c r="F93" s="18" t="s">
         <v>36</v>
@@ -6993,7 +7092,7 @@
       <c r="C95" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D95" s="5"/>
+      <c r="D95" s="14"/>
       <c r="E95" s="5"/>
       <c r="F95" s="15" t="s">
         <v>22</v>
@@ -7033,7 +7132,7 @@
       <c r="C96" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D96" s="21"/>
+      <c r="D96" s="14"/>
       <c r="E96" s="21"/>
       <c r="F96" s="18" t="s">
         <v>36</v>
@@ -7069,7 +7168,9 @@
       <c r="C97" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D97" s="14"/>
+      <c r="D97" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E97" s="14"/>
       <c r="F97" s="18" t="s">
         <v>36</v>
@@ -7143,7 +7244,7 @@
       <c r="C99" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="D99" s="21"/>
+      <c r="D99" s="14"/>
       <c r="E99" s="21"/>
       <c r="F99" s="15" t="s">
         <v>19</v>
@@ -7179,7 +7280,7 @@
       <c r="C100" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D100" s="5"/>
+      <c r="D100" s="14"/>
       <c r="E100" s="5"/>
       <c r="F100" s="15" t="s">
         <v>22</v>
@@ -7217,7 +7318,9 @@
       <c r="C101" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D101" s="14"/>
+      <c r="D101" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E101" s="14"/>
       <c r="F101" s="18" t="s">
         <v>36</v>
@@ -7363,9 +7466,11 @@
         <v>173</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D105" s="14"/>
+        <v>267</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E105" s="14"/>
       <c r="F105" s="18" t="s">
         <v>36</v>
@@ -7481,7 +7586,7 @@
       <c r="C108" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="D108" s="21"/>
+      <c r="D108" s="14"/>
       <c r="E108" s="21"/>
       <c r="F108" s="18" t="s">
         <v>36</v>
@@ -7559,7 +7664,7 @@
       <c r="C110" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D110" s="5"/>
+      <c r="D110" s="14"/>
       <c r="E110" s="5"/>
       <c r="F110" s="15" t="s">
         <v>19</v>
@@ -7749,9 +7854,11 @@
         <v>184</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D115" s="14"/>
+        <v>268</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E115" s="14"/>
       <c r="F115" s="18" t="s">
         <v>36</v>
@@ -7789,7 +7896,7 @@
       <c r="C116" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D116" s="21"/>
+      <c r="D116" s="14"/>
       <c r="E116" s="21"/>
       <c r="F116" s="15" t="s">
         <v>22</v>
@@ -7983,7 +8090,9 @@
       <c r="C121" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D121" s="14"/>
+      <c r="D121" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E121" s="14"/>
       <c r="F121" s="18" t="s">
         <v>36</v>
@@ -8021,9 +8130,11 @@
         <v>150</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D122" s="14"/>
+        <v>266</v>
+      </c>
+      <c r="D122" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E122" s="14"/>
       <c r="F122" s="18" t="s">
         <v>36</v>
@@ -8061,7 +8172,7 @@
       <c r="C123" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D123" s="21"/>
+      <c r="D123" s="14"/>
       <c r="E123" s="21"/>
       <c r="F123" s="15" t="s">
         <v>22</v>
@@ -8097,7 +8208,7 @@
       <c r="C124" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D124" s="21"/>
+      <c r="D124" s="14"/>
       <c r="E124" s="21"/>
       <c r="F124" s="15" t="s">
         <v>22</v>
@@ -8137,7 +8248,7 @@
       <c r="C125" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="D125" s="21"/>
+      <c r="D125" s="14"/>
       <c r="E125" s="21"/>
       <c r="F125" s="15" t="s">
         <v>30</v>
@@ -8171,7 +8282,9 @@
       <c r="C126" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D126" s="14"/>
+      <c r="D126" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E126" s="14"/>
       <c r="F126" s="18" t="s">
         <v>36</v>
@@ -8201,7 +8314,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="30" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A127" s="12">
         <v>126</v>
       </c>
@@ -8273,7 +8386,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="30" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:16" ht="15" x14ac:dyDescent="0.15">
       <c r="A129" s="12">
         <v>128</v>
       </c>
@@ -8323,7 +8436,7 @@
       <c r="C130" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D130" s="21"/>
+      <c r="D130" s="14"/>
       <c r="E130" s="21"/>
       <c r="F130" s="15" t="s">
         <v>22</v>
@@ -8435,7 +8548,7 @@
       <c r="C133" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D133" s="21"/>
+      <c r="D133" s="14"/>
       <c r="E133" s="21"/>
       <c r="F133" s="15" t="s">
         <v>22</v>
@@ -8513,9 +8626,11 @@
         <v>203</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D135" s="14"/>
+        <v>264</v>
+      </c>
+      <c r="D135" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E135" s="14"/>
       <c r="F135" s="15" t="s">
         <v>17</v>
@@ -8553,7 +8668,7 @@
       <c r="C136" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="D136" s="21"/>
+      <c r="D136" s="14"/>
       <c r="E136" s="21"/>
       <c r="F136" s="15" t="s">
         <v>22</v>
@@ -8665,9 +8780,11 @@
         <v>207</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D139" s="14"/>
+        <v>265</v>
+      </c>
+      <c r="D139" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="E139" s="14"/>
       <c r="F139" s="18" t="s">
         <v>36</v>
@@ -8735,7 +8852,29 @@
         <v>2024</v>
       </c>
     </row>
+    <row r="141" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="D141" s="14"/>
+    </row>
+    <row r="142" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="D142" s="14"/>
+    </row>
+    <row r="143" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="D143" s="14"/>
+    </row>
+    <row r="144" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="D144" s="14"/>
+    </row>
+    <row r="145" spans="4:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="D145" s="14"/>
+    </row>
+    <row r="146" spans="4:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="D146" s="14"/>
+    </row>
+    <row r="147" spans="4:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="D147" s="14"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:R140" xr:uid="{C9F364D8-7C39-9F42-8917-7C47B6C1B156}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>